<commit_message>
Updated for SAP S/4 HANA 2023 (new version).
</commit_message>
<xml_diff>
--- a/E2E/Default.xlsx
+++ b/E2E/Default.xlsx
@@ -55,6 +55,9 @@
     <t>CHROME</t>
   </si>
   <si>
+    <t>EWMS4-01</t>
+  </si>
+  <si>
     <t>OrderQuantity</t>
   </si>
   <si>
@@ -68,9 +71,6 @@
   </si>
   <si>
     <t>BillingNumber</t>
-  </si>
-  <si>
-    <t>EWMS4-02</t>
   </si>
   <si>
     <t>UnitOfMeasure</t>
@@ -253,6 +253,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -263,7 +272,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -283,17 +294,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -303,15 +303,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,60 +630,60 @@
     <col min="12" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="4" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="14.95" s="6" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="5"/>
     </row>
   </sheetData>
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -1031,32 +1031,32 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="4" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="14.95" s="6" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>